<commit_message>
Updated for Pope Leo XIV
</commit_message>
<xml_diff>
--- a/data/popes.xlsx
+++ b/data/popes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Chungus/local_tasks/programming/popes/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thejustintung/Desktop/programming/popes_by_order/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE2BE21-5333-E640-9ABD-58DA0C37F6F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74B231A-AEC3-1648-9435-CA19E1937E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="1151">
   <si>
     <t>Pontificate</t>
   </si>
@@ -3470,13 +3470,42 @@
   </si>
   <si>
     <t>Gregory XII</t>
+  </si>
+  <si>
+    <t>Leo XIV</t>
+  </si>
+  <si>
+    <r>
+      <t>LEO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Quartus Decimus</t>
+    </r>
+  </si>
+  <si>
+    <t>Robert Francis Prevost, O.S.A.</t>
+  </si>
+  <si>
+    <t>Chicago, Illinois, United States</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>First American Pope</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3525,6 +3554,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3546,7 +3588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3572,6 +3614,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3914,10 +3962,10 @@
   <dimension ref="A1:M273"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B222" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B267" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N228" sqref="N228"/>
+      <selection pane="bottomRight" activeCell="C272" sqref="C272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11810,7 +11858,7 @@
         <v>2013</v>
       </c>
       <c r="C271">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D271" s="2" t="s">
         <v>1100</v>
@@ -11838,6 +11886,44 @@
       </c>
       <c r="M271" s="7" t="s">
         <v>1133</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A272" s="9">
+        <v>45785</v>
+      </c>
+      <c r="B272">
+        <v>2025</v>
+      </c>
+      <c r="C272" s="3">
+        <v>2025</v>
+      </c>
+      <c r="D272" s="3" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E272" s="10" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F272" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G272" s="3" t="s">
+        <v>1148</v>
+      </c>
+      <c r="H272" s="3" t="s">
+        <v>1149</v>
+      </c>
+      <c r="I272">
+        <v>69</v>
+      </c>
+      <c r="K272" s="3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="L272" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="M272" s="3" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="13" x14ac:dyDescent="0.15">

</xml_diff>